<commit_message>
fix the introduction slide
</commit_message>
<xml_diff>
--- a/Program.xlsx
+++ b/Program.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/matteo_francia2_studio_unibo_it/Documents/teaching-bigdata/AA2425-unibo-bigdataandcloudplatforms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/matteo_francia2_studio_unibo_it/Documents/teaching-bigdata/AA2526-unibo-bigdataandcloudplatforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{F7F973B8-4F16-4EF1-8487-709103825833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB6EFB66-5367-4513-9297-F271FA0E0136}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{F7F973B8-4F16-4EF1-8487-709103825833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CA14C93-6E9B-4755-AB5B-7E5EEA01024C}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="15990" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Calendar AA 2324" sheetId="2" r:id="rId1"/>
-    <sheet name="Calendar AA 2223" sheetId="1" r:id="rId2"/>
+    <sheet name="Calendar AA 2526" sheetId="3" r:id="rId1"/>
+    <sheet name="Calendar AA 2425" sheetId="2" r:id="rId2"/>
+    <sheet name="Calendar AA 2223" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="60">
   <si>
     <t>Lab</t>
   </si>
@@ -212,6 +213,9 @@
   </si>
   <si>
     <t>AULA 2.4, 2h (11-13)</t>
+  </si>
+  <si>
+    <t>Seminar: TBD</t>
   </si>
 </sst>
 </file>
@@ -415,7 +419,14 @@
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -705,28 +716,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FA0065-A3C8-4E4D-B5EC-36CCF9E12688}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE48BDE-AF85-4F5A-91B1-CBAD698B62C1}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.90625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" style="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.1796875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.21875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -758,13 +769,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>45580</v>
+        <v>45572</v>
       </c>
       <c r="B2" s="23">
         <f>WEEKDAY(A2)-1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>48</v>
@@ -789,14 +800,14 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <f>A2</f>
-        <v>45580</v>
+        <v>45572</v>
       </c>
       <c r="B3" s="23">
         <f t="shared" ref="B3:B21" si="0">WEEKDAY(A3)-1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>49</v>
@@ -824,17 +835,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <f>A3+7</f>
-        <v>45587</v>
+        <v>45579</v>
       </c>
       <c r="B4" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1</v>
@@ -859,23 +870,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <f>A3+8</f>
-        <v>45588</v>
+        <f>A4+7</f>
+        <v>45586</v>
       </c>
       <c r="B5" s="23">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>54</v>
@@ -888,19 +899,20 @@
       </c>
       <c r="I5" s="10">
         <f>SUM($E$2:E5)/$E$23</f>
-        <v>0.3</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="J5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
-        <v>45601</v>
+        <f>A5+7</f>
+        <v>45593</v>
       </c>
       <c r="B6" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>48</v>
@@ -922,20 +934,20 @@
       </c>
       <c r="I6" s="10">
         <f>SUM($E$2:E6)/$E$23</f>
-        <v>0.36666666666666664</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <f>A6</f>
-        <v>45601</v>
+        <v>45593</v>
       </c>
       <c r="B7" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>49</v>
@@ -957,17 +969,17 @@
       </c>
       <c r="I7" s="10">
         <f>SUM($E$2:E7)/$E$23</f>
-        <v>0.43333333333333335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <f>A7+7</f>
-        <v>45608</v>
+        <v>45600</v>
       </c>
       <c r="B8" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>48</v>
@@ -989,17 +1001,17 @@
       </c>
       <c r="I8" s="10">
         <f>SUM($E$2:E8)/$E$23</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <f>A8</f>
-        <v>45608</v>
+        <v>45600</v>
       </c>
       <c r="B9" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>49</v>
@@ -1021,20 +1033,20 @@
       </c>
       <c r="I9" s="10">
         <f>SUM($E$2:E9)/$E$23</f>
-        <v>0.56666666666666665</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="J9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <f>A9+7</f>
-        <v>45615</v>
+        <v>45607</v>
       </c>
       <c r="B10" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>48</v>
@@ -1056,20 +1068,20 @@
       </c>
       <c r="I10" s="10">
         <f>SUM($E$2:E10)/$E$23</f>
-        <v>0.6333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="J10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <f>A10</f>
-        <v>45615</v>
+        <v>45607</v>
       </c>
       <c r="B11" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>49</v>
@@ -1091,17 +1103,17 @@
       </c>
       <c r="I11" s="10">
         <f>SUM($E$2:E11)/$E$23</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <f>A11+7</f>
-        <v>45622</v>
+        <v>45614</v>
       </c>
       <c r="B12" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>48</v>
@@ -1113,7 +1125,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G12" s="17">
         <v>2</v>
@@ -1123,17 +1135,17 @@
       </c>
       <c r="I12" s="10">
         <f>SUM($E$2:E12)/$E$23</f>
-        <v>0.76666666666666672</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <f>A12</f>
-        <v>45622</v>
+        <v>45614</v>
       </c>
       <c r="B13" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>49</v>
@@ -1153,17 +1165,17 @@
       </c>
       <c r="I13" s="10">
         <f>SUM($E$2:E13)/$E$23</f>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <f>A13+7</f>
-        <v>45629</v>
+        <v>45621</v>
       </c>
       <c r="B14" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>48</v>
@@ -1175,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G14" s="17">
         <v>3</v>
@@ -1185,20 +1197,20 @@
       </c>
       <c r="I14" s="10">
         <f>SUM($E$2:E14)/$E$23</f>
-        <v>0.9</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="J14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <f>A14</f>
-        <v>45629</v>
+        <v>45621</v>
       </c>
       <c r="B15" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>58</v>
@@ -1216,20 +1228,20 @@
       <c r="H15" s="13"/>
       <c r="I15" s="10">
         <f>SUM($E$2:E15)/$E$23</f>
-        <v>0.96666666666666667</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="J15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <f>A15+7</f>
-        <v>45636</v>
+        <v>45628</v>
       </c>
       <c r="B16" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>48</v>
@@ -1246,17 +1258,17 @@
       <c r="H16" s="16"/>
       <c r="I16" s="10">
         <f>SUM($E$2:E17)/$E$23</f>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <f>A16</f>
-        <v>45636</v>
+        <v>45628</v>
       </c>
       <c r="B17" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>49</v>
@@ -1276,17 +1288,17 @@
       <c r="H17" s="13"/>
       <c r="I17" s="10">
         <f>SUM($E$2:E17)/$E$23</f>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <f>A17+7</f>
-        <v>45643</v>
+        <v>45635</v>
       </c>
       <c r="B18" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>48</v>
@@ -1301,17 +1313,17 @@
       <c r="H18" s="16"/>
       <c r="I18" s="10">
         <f>SUM($E$2:E18)/$E$23</f>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <f>A18</f>
-        <v>45643</v>
+        <v>45635</v>
       </c>
       <c r="B19" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>49</v>
@@ -1326,17 +1338,17 @@
       <c r="H19" s="15"/>
       <c r="I19" s="10">
         <f>SUM($E$2:E19)/$E$23</f>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <f>A19+7</f>
-        <v>45650</v>
+        <v>45642</v>
       </c>
       <c r="B20" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>48</v>
@@ -1348,14 +1360,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <f>A20</f>
-        <v>45650</v>
+        <v>45642</v>
       </c>
       <c r="B21" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>49</v>
@@ -1367,16 +1379,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E22" s="2">
         <f>SUM(E2:E21)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1384,7 +1396,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E32" s="24"/>
     </row>
   </sheetData>
@@ -1404,8 +1416,721 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1 E23 D23:D1048576 D1:D15 D17:D19">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="F1 D1:D15 D17:D19 E23 D23:D1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Theory"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{A52683A8-AE0E-47A6-9596-30CB0C91B49A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FA0065-A3C8-4E4D-B5EC-36CCF9E12688}">
+  <dimension ref="A1:J32"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.21875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>45580</v>
+      </c>
+      <c r="B2" s="23">
+        <f>WEEKDAY(A2)-1</f>
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22">
+        <v>2</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="17">
+        <v>3</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10">
+        <f>SUM($E$2:E2)/$E$23</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <f>A2</f>
+        <v>45580</v>
+      </c>
+      <c r="B3" s="23">
+        <f t="shared" ref="B3:B21" si="0">WEEKDAY(A3)-1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22">
+        <v>2</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="17">
+        <v>2</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="10">
+        <f>SUM($E$2:E3)/$E$23</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <f>A3+7</f>
+        <v>45587</v>
+      </c>
+      <c r="B4" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="10">
+        <f>SUM($E$2:E4)/$E$23</f>
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <f>A3+8</f>
+        <v>45588</v>
+      </c>
+      <c r="B5" s="23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="22">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="17">
+        <v>3</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="10">
+        <f>SUM($E$2:E5)/$E$23</f>
+        <v>0.3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>45601</v>
+      </c>
+      <c r="B6" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22">
+        <v>2</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17">
+        <v>2</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="10">
+        <f>SUM($E$2:E6)/$E$23</f>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <f>A6</f>
+        <v>45601</v>
+      </c>
+      <c r="B7" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="22">
+        <v>2</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="17">
+        <v>2</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="10">
+        <f>SUM($E$2:E7)/$E$23</f>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <f>A7+7</f>
+        <v>45608</v>
+      </c>
+      <c r="B8" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="22">
+        <v>2</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="17">
+        <v>3</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="10">
+        <f>SUM($E$2:E8)/$E$23</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <f>A8</f>
+        <v>45608</v>
+      </c>
+      <c r="B9" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="22">
+        <v>2</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="17">
+        <v>2</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="10">
+        <f>SUM($E$2:E9)/$E$23</f>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <f>A9+7</f>
+        <v>45615</v>
+      </c>
+      <c r="B10" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22">
+        <v>2</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="17">
+        <v>2</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="10">
+        <f>SUM($E$2:E10)/$E$23</f>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <f>A10</f>
+        <v>45615</v>
+      </c>
+      <c r="B11" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="22">
+        <v>2</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="17">
+        <v>3</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="10">
+        <f>SUM($E$2:E11)/$E$23</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <f>A11+7</f>
+        <v>45622</v>
+      </c>
+      <c r="B12" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="22">
+        <v>2</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="17">
+        <v>2</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="10">
+        <f>SUM($E$2:E12)/$E$23</f>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f>A12</f>
+        <v>45622</v>
+      </c>
+      <c r="B13" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="22">
+        <v>2</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="17">
+        <v>2</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="10">
+        <f>SUM($E$2:E13)/$E$23</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <f>A13+7</f>
+        <v>45629</v>
+      </c>
+      <c r="B14" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="22">
+        <v>2</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="17">
+        <v>3</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="10">
+        <f>SUM($E$2:E14)/$E$23</f>
+        <v>0.9</v>
+      </c>
+      <c r="J14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <f>A14</f>
+        <v>45629</v>
+      </c>
+      <c r="B15" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="22">
+        <v>2</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="10">
+        <f>SUM($E$2:E15)/$E$23</f>
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="J15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <f>A15+7</f>
+        <v>45636</v>
+      </c>
+      <c r="B16" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="10">
+        <f>SUM($E$2:E17)/$E$23</f>
+        <v>1.0333333333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <f>A16</f>
+        <v>45636</v>
+      </c>
+      <c r="B17" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="22">
+        <v>2</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="10">
+        <f>SUM($E$2:E17)/$E$23</f>
+        <v>1.0333333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <f>A17+7</f>
+        <v>45643</v>
+      </c>
+      <c r="B18" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="10">
+        <f>SUM($E$2:E18)/$E$23</f>
+        <v>1.0333333333333334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <f>A18</f>
+        <v>45643</v>
+      </c>
+      <c r="B19" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="10">
+        <f>SUM($E$2:E19)/$E$23</f>
+        <v>1.0333333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <f>A19+7</f>
+        <v>45650</v>
+      </c>
+      <c r="B20" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <f>A20</f>
+        <v>45650</v>
+      </c>
+      <c r="B21" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="2">
+        <f>SUM(E2:E21)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E32" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1 D1:D15 D17:D19 E23 D23:D1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Theory"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1417,7 +2142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
@@ -1425,19 +2150,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.81640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="9"/>
+    <col min="4" max="4" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" style="9"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1463,7 +2188,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>44860</v>
       </c>
@@ -1491,7 +2216,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>44860</v>
       </c>
@@ -1515,7 +2240,7 @@
       </c>
       <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>44867</v>
       </c>
@@ -1541,7 +2266,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>44867</v>
       </c>
@@ -1569,7 +2294,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>44874</v>
       </c>
@@ -1595,7 +2320,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>44874</v>
       </c>
@@ -1623,7 +2348,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>44881</v>
       </c>
@@ -1649,7 +2374,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>44881</v>
       </c>
@@ -1677,7 +2402,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>44888</v>
       </c>
@@ -1702,7 +2427,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>44888</v>
       </c>
@@ -1727,7 +2452,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>44893</v>
       </c>
@@ -1753,7 +2478,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>44895</v>
       </c>
@@ -1777,7 +2502,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>44895</v>
       </c>
@@ -1799,7 +2524,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>44900</v>
       </c>
@@ -1825,7 +2550,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>44902</v>
       </c>
@@ -1851,7 +2576,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>44907</v>
       </c>
@@ -1877,7 +2602,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1906,7 +2631,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Theory"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix: update case study
</commit_message>
<xml_diff>
--- a/Program.xlsx
+++ b/Program.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/matteo_francia2_studio_unibo_it/Documents/teaching-bigdata/AA2526-unibo-bigdataandcloudplatforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{F7F973B8-4F16-4EF1-8487-709103825833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CA14C93-6E9B-4755-AB5B-7E5EEA01024C}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{F7F973B8-4F16-4EF1-8487-709103825833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE98AEE8-D25D-47FB-BECA-AB4C98B0EE5B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="15990" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar AA 2526" sheetId="3" r:id="rId1"/>
@@ -31,12 +31,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="61">
   <si>
     <t>Lab</t>
   </si>
@@ -216,13 +219,16 @@
   </si>
   <si>
     <t>Seminar: TBD</t>
+  </si>
+  <si>
+    <t>Towards data platforms (until case study on data profiling)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +287,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -333,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,6 +426,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -720,24 +736,24 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" style="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.21875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -769,7 +785,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45572</v>
       </c>
@@ -800,7 +816,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>A2</f>
         <v>45572</v>
@@ -819,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G3" s="17">
         <v>2</v>
@@ -835,7 +851,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f>A3+7</f>
         <v>45579</v>
@@ -870,7 +886,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f>A4+7</f>
         <v>45586</v>
@@ -888,7 +904,7 @@
       <c r="E5" s="22">
         <v>2</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="28" t="s">
         <v>54</v>
       </c>
       <c r="G5" s="17">
@@ -905,7 +921,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f>A5+7</f>
         <v>45593</v>
@@ -923,7 +939,7 @@
       <c r="E6" s="22">
         <v>2</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="28" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="17">
@@ -940,7 +956,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <f>A6</f>
         <v>45593</v>
@@ -958,7 +974,7 @@
       <c r="E7" s="22">
         <v>2</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="28" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="17">
@@ -972,7 +988,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f>A7+7</f>
         <v>45600</v>
@@ -990,7 +1006,7 @@
       <c r="E8" s="22">
         <v>2</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="28" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="17">
@@ -1004,7 +1020,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f>A8</f>
         <v>45600</v>
@@ -1022,7 +1038,7 @@
       <c r="E9" s="22">
         <v>2</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="28" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="17">
@@ -1039,7 +1055,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <f>A9+7</f>
         <v>45607</v>
@@ -1057,7 +1073,7 @@
       <c r="E10" s="22">
         <v>2</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="28" t="s">
         <v>55</v>
       </c>
       <c r="G10" s="17">
@@ -1074,7 +1090,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <f>A10</f>
         <v>45607</v>
@@ -1092,7 +1108,7 @@
       <c r="E11" s="22">
         <v>2</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="28" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="17">
@@ -1106,7 +1122,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f>A11+7</f>
         <v>45614</v>
@@ -1138,7 +1154,7 @@
         <v>0.73333333333333328</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f>A12</f>
         <v>45614</v>
@@ -1168,7 +1184,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f>A13+7</f>
         <v>45621</v>
@@ -1203,7 +1219,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f>A14</f>
         <v>45621</v>
@@ -1234,7 +1250,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f>A15+7</f>
         <v>45628</v>
@@ -1261,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f>A16</f>
         <v>45628</v>
@@ -1291,7 +1307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f>A17+7</f>
         <v>45635</v>
@@ -1316,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f>A18</f>
         <v>45635</v>
@@ -1341,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <f>A19+7</f>
         <v>45642</v>
@@ -1360,7 +1376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <f>A20</f>
         <v>45642</v>
@@ -1379,7 +1395,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1388,7 +1404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1396,720 +1412,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E32" s="24"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1 D1:D15 D17:D19 E23 D23:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Theory"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{A52683A8-AE0E-47A6-9596-30CB0C91B49A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FA0065-A3C8-4E4D-B5EC-36CCF9E12688}">
-  <dimension ref="A1:J32"/>
-  <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" style="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.21875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>45580</v>
-      </c>
-      <c r="B2" s="23">
-        <f>WEEKDAY(A2)-1</f>
-        <v>2</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="22">
-        <v>2</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="17">
-        <v>3</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="10">
-        <f>SUM($E$2:E2)/$E$23</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <f>A2</f>
-        <v>45580</v>
-      </c>
-      <c r="B3" s="23">
-        <f t="shared" ref="B3:B21" si="0">WEEKDAY(A3)-1</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="22">
-        <v>2</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="17">
-        <v>2</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="10">
-        <f>SUM($E$2:E3)/$E$23</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="J3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <f>A3+7</f>
-        <v>45587</v>
-      </c>
-      <c r="B4" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="22">
-        <v>2</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="17">
-        <v>2</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="10">
-        <f>SUM($E$2:E4)/$E$23</f>
-        <v>0.2</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <f>A3+8</f>
-        <v>45588</v>
-      </c>
-      <c r="B5" s="23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="22">
-        <v>3</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="17">
-        <v>3</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="10">
-        <f>SUM($E$2:E5)/$E$23</f>
-        <v>0.3</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>45601</v>
-      </c>
-      <c r="B6" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="22">
-        <v>2</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="17">
-        <v>2</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="10">
-        <f>SUM($E$2:E6)/$E$23</f>
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <f>A6</f>
-        <v>45601</v>
-      </c>
-      <c r="B7" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="22">
-        <v>2</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="17">
-        <v>2</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="10">
-        <f>SUM($E$2:E7)/$E$23</f>
-        <v>0.43333333333333335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <f>A7+7</f>
-        <v>45608</v>
-      </c>
-      <c r="B8" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="22">
-        <v>2</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="17">
-        <v>3</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="10">
-        <f>SUM($E$2:E8)/$E$23</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <f>A8</f>
-        <v>45608</v>
-      </c>
-      <c r="B9" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="22">
-        <v>2</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="17">
-        <v>2</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="10">
-        <f>SUM($E$2:E9)/$E$23</f>
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="J9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <f>A9+7</f>
-        <v>45615</v>
-      </c>
-      <c r="B10" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="22">
-        <v>2</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="17">
-        <v>2</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="10">
-        <f>SUM($E$2:E10)/$E$23</f>
-        <v>0.6333333333333333</v>
-      </c>
-      <c r="J10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <f>A10</f>
-        <v>45615</v>
-      </c>
-      <c r="B11" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="22">
-        <v>2</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="17">
-        <v>3</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="10">
-        <f>SUM($E$2:E11)/$E$23</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <f>A11+7</f>
-        <v>45622</v>
-      </c>
-      <c r="B12" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="22">
-        <v>2</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="17">
-        <v>2</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="10">
-        <f>SUM($E$2:E12)/$E$23</f>
-        <v>0.76666666666666672</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <f>A12</f>
-        <v>45622</v>
-      </c>
-      <c r="B13" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="22">
-        <v>2</v>
-      </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="17">
-        <v>2</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="10">
-        <f>SUM($E$2:E13)/$E$23</f>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <f>A13+7</f>
-        <v>45629</v>
-      </c>
-      <c r="B14" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="22">
-        <v>2</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="17">
-        <v>3</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="10">
-        <f>SUM($E$2:E14)/$E$23</f>
-        <v>0.9</v>
-      </c>
-      <c r="J14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <f>A14</f>
-        <v>45629</v>
-      </c>
-      <c r="B15" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="22">
-        <v>2</v>
-      </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="10">
-        <f>SUM($E$2:E15)/$E$23</f>
-        <v>0.96666666666666667</v>
-      </c>
-      <c r="J15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <f>A15+7</f>
-        <v>45636</v>
-      </c>
-      <c r="B16" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="10">
-        <f>SUM($E$2:E17)/$E$23</f>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <f>A16</f>
-        <v>45636</v>
-      </c>
-      <c r="B17" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="22">
-        <v>2</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="10">
-        <f>SUM($E$2:E17)/$E$23</f>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <f>A17+7</f>
-        <v>45643</v>
-      </c>
-      <c r="B18" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="10">
-        <f>SUM($E$2:E18)/$E$23</f>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <f>A18</f>
-        <v>45643</v>
-      </c>
-      <c r="B19" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="10">
-        <f>SUM($E$2:E19)/$E$23</f>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <f>A19+7</f>
-        <v>45650</v>
-      </c>
-      <c r="B20" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
-        <f>A20</f>
-        <v>45650</v>
-      </c>
-      <c r="B21" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="2">
-        <f>SUM(E2:E21)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E32" s="24"/>
     </row>
   </sheetData>
@@ -2135,6 +1438,719 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{A52683A8-AE0E-47A6-9596-30CB0C91B49A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FA0065-A3C8-4E4D-B5EC-36CCF9E12688}">
+  <dimension ref="A1:J32"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>45580</v>
+      </c>
+      <c r="B2" s="23">
+        <f>WEEKDAY(A2)-1</f>
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22">
+        <v>2</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="17">
+        <v>3</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10">
+        <f>SUM($E$2:E2)/$E$23</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <f>A2</f>
+        <v>45580</v>
+      </c>
+      <c r="B3" s="23">
+        <f t="shared" ref="B3:B21" si="0">WEEKDAY(A3)-1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22">
+        <v>2</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="17">
+        <v>2</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="10">
+        <f>SUM($E$2:E3)/$E$23</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <f>A3+7</f>
+        <v>45587</v>
+      </c>
+      <c r="B4" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="10">
+        <f>SUM($E$2:E4)/$E$23</f>
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <f>A3+8</f>
+        <v>45588</v>
+      </c>
+      <c r="B5" s="23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="22">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="17">
+        <v>3</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="10">
+        <f>SUM($E$2:E5)/$E$23</f>
+        <v>0.3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>45601</v>
+      </c>
+      <c r="B6" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22">
+        <v>2</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17">
+        <v>2</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="10">
+        <f>SUM($E$2:E6)/$E$23</f>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <f>A6</f>
+        <v>45601</v>
+      </c>
+      <c r="B7" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="22">
+        <v>2</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="17">
+        <v>2</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="10">
+        <f>SUM($E$2:E7)/$E$23</f>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <f>A7+7</f>
+        <v>45608</v>
+      </c>
+      <c r="B8" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="22">
+        <v>2</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="17">
+        <v>3</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="10">
+        <f>SUM($E$2:E8)/$E$23</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <f>A8</f>
+        <v>45608</v>
+      </c>
+      <c r="B9" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="22">
+        <v>2</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="17">
+        <v>2</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="10">
+        <f>SUM($E$2:E9)/$E$23</f>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <f>A9+7</f>
+        <v>45615</v>
+      </c>
+      <c r="B10" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22">
+        <v>2</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="17">
+        <v>2</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="10">
+        <f>SUM($E$2:E10)/$E$23</f>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <f>A10</f>
+        <v>45615</v>
+      </c>
+      <c r="B11" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="22">
+        <v>2</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="17">
+        <v>3</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="10">
+        <f>SUM($E$2:E11)/$E$23</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f>A11+7</f>
+        <v>45622</v>
+      </c>
+      <c r="B12" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="22">
+        <v>2</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="17">
+        <v>2</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="10">
+        <f>SUM($E$2:E12)/$E$23</f>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f>A12</f>
+        <v>45622</v>
+      </c>
+      <c r="B13" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="22">
+        <v>2</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="17">
+        <v>2</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="10">
+        <f>SUM($E$2:E13)/$E$23</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <f>A13+7</f>
+        <v>45629</v>
+      </c>
+      <c r="B14" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="22">
+        <v>2</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="17">
+        <v>3</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="10">
+        <f>SUM($E$2:E14)/$E$23</f>
+        <v>0.9</v>
+      </c>
+      <c r="J14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f>A14</f>
+        <v>45629</v>
+      </c>
+      <c r="B15" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="22">
+        <v>2</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="10">
+        <f>SUM($E$2:E15)/$E$23</f>
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="J15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f>A15+7</f>
+        <v>45636</v>
+      </c>
+      <c r="B16" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="10">
+        <f>SUM($E$2:E17)/$E$23</f>
+        <v>1.0333333333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f>A16</f>
+        <v>45636</v>
+      </c>
+      <c r="B17" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="22">
+        <v>2</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="10">
+        <f>SUM($E$2:E17)/$E$23</f>
+        <v>1.0333333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <f>A17+7</f>
+        <v>45643</v>
+      </c>
+      <c r="B18" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="10">
+        <f>SUM($E$2:E18)/$E$23</f>
+        <v>1.0333333333333334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <f>A18</f>
+        <v>45643</v>
+      </c>
+      <c r="B19" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="10">
+        <f>SUM($E$2:E19)/$E$23</f>
+        <v>1.0333333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <f>A19+7</f>
+        <v>45650</v>
+      </c>
+      <c r="B20" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <f>A20</f>
+        <v>45650</v>
+      </c>
+      <c r="B21" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="2">
+        <f>SUM(E2:E21)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E32" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1 D1:D15 D17:D19 E23 D23:D1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Theory"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{922831C9-06CF-4175-BF25-76682238DB37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2150,19 +2166,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" style="9"/>
+    <col min="4" max="4" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="9"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2188,7 +2204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>44860</v>
       </c>
@@ -2216,7 +2232,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>44860</v>
       </c>
@@ -2240,7 +2256,7 @@
       </c>
       <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>44867</v>
       </c>
@@ -2266,7 +2282,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>44867</v>
       </c>
@@ -2294,7 +2310,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>44874</v>
       </c>
@@ -2320,7 +2336,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>44874</v>
       </c>
@@ -2348,7 +2364,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>44881</v>
       </c>
@@ -2374,7 +2390,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>44881</v>
       </c>
@@ -2402,7 +2418,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>44888</v>
       </c>
@@ -2427,7 +2443,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>44888</v>
       </c>
@@ -2452,7 +2468,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>44893</v>
       </c>
@@ -2478,7 +2494,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>44895</v>
       </c>
@@ -2502,7 +2518,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>44895</v>
       </c>
@@ -2524,7 +2540,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>44900</v>
       </c>
@@ -2550,7 +2566,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>44902</v>
       </c>
@@ -2576,7 +2592,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>44907</v>
       </c>
@@ -2602,7 +2618,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="5" t="s">
         <v>2</v>
       </c>
@@ -2631,7 +2647,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Theory"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix: graph data model
</commit_message>
<xml_diff>
--- a/Program.xlsx
+++ b/Program.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/matteo_francia2_studio_unibo_it/Documents/teaching-bigdata/AA2526-unibo-bigdataandcloudplatforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{F7F973B8-4F16-4EF1-8487-709103825833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE98AEE8-D25D-47FB-BECA-AB4C98B0EE5B}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{F7F973B8-4F16-4EF1-8487-709103825833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{638E8B95-7E36-46BC-A236-0B95EA2E2716}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15990" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar AA 2526" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="70">
   <si>
     <t>Lab</t>
   </si>
@@ -218,10 +218,37 @@
     <t>AULA 2.4, 2h (11-13)</t>
   </si>
   <si>
-    <t>Seminar: TBD</t>
-  </si>
-  <si>
     <t>Towards data platforms (until case study on data profiling)</t>
+  </si>
+  <si>
+    <t>Seminar: Technogym</t>
+  </si>
+  <si>
+    <t>Seminar: UniBO (Manuele Pasini)</t>
+  </si>
+  <si>
+    <t>Towards data platforms (until hera seminar)</t>
+  </si>
+  <si>
+    <t>Introduction, Towards data platforms</t>
+  </si>
+  <si>
+    <t>Towards data platforms (until lakehouse?)</t>
+  </si>
+  <si>
+    <t>Cloud (Storage)</t>
+  </si>
+  <si>
+    <t>Cloud (Computing)</t>
+  </si>
+  <si>
+    <t>Cloud (Migration)</t>
+  </si>
+  <si>
+    <t>Integrated Lab</t>
+  </si>
+  <si>
+    <t>Towards data platforms, NoSQL (until CAP)</t>
   </si>
 </sst>
 </file>
@@ -289,13 +316,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="2" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +359,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -346,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,7 +460,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -733,27 +775,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE48BDE-AF85-4F5A-91B1-CBAD698B62C1}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" style="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.26953125" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -772,20 +812,14 @@
       <c r="F1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45572</v>
       </c>
@@ -803,20 +837,14 @@
         <v>2</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="17">
-        <v>3</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="10">
+        <v>63</v>
+      </c>
+      <c r="G2" s="22">
         <f>SUM($E$2:E2)/$E$23</f>
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <f>A2</f>
         <v>45572</v>
@@ -835,23 +863,14 @@
         <v>2</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="17">
-        <v>2</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="10">
+        <v>64</v>
+      </c>
+      <c r="G3" s="22">
         <f>SUM($E$2:E3)/$E$23</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="J3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <f>A3+7</f>
         <v>45579</v>
@@ -870,23 +889,15 @@
         <v>2</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="17">
-        <v>2</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="10">
+        <v>59</v>
+      </c>
+      <c r="G4" s="22">
         <f>SUM($E$2:E4)/$E$23</f>
         <v>0.2</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <f>A4+7</f>
         <v>45586</v>
@@ -904,24 +915,15 @@
       <c r="E5" s="22">
         <v>2</v>
       </c>
-      <c r="F5" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="17">
-        <v>3</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="10">
+      <c r="F5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="22">
         <f>SUM($E$2:E5)/$E$23</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="J5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <f>A5+7</f>
         <v>45593</v>
@@ -939,24 +941,15 @@
       <c r="E6" s="22">
         <v>2</v>
       </c>
-      <c r="F6" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="17">
-        <v>2</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="F6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="22">
         <f>SUM($E$2:E6)/$E$23</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <f>A6</f>
         <v>45593</v>
@@ -974,21 +967,15 @@
       <c r="E7" s="22">
         <v>2</v>
       </c>
-      <c r="F7" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="17">
-        <v>2</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="10">
+      <c r="F7" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="22">
         <f>SUM($E$2:E7)/$E$23</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <f>A7+7</f>
         <v>45600</v>
@@ -1006,21 +993,15 @@
       <c r="E8" s="22">
         <v>2</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="17">
-        <v>3</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="F8" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="22">
         <f>SUM($E$2:E8)/$E$23</f>
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <f>A8</f>
         <v>45600</v>
@@ -1038,24 +1019,15 @@
       <c r="E9" s="22">
         <v>2</v>
       </c>
-      <c r="F9" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="17">
-        <v>2</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="10">
+      <c r="F9" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="22">
         <f>SUM($E$2:E9)/$E$23</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="J9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <f>A9+7</f>
         <v>45607</v>
@@ -1073,24 +1045,15 @@
       <c r="E10" s="22">
         <v>2</v>
       </c>
-      <c r="F10" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="17">
-        <v>2</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="10">
+      <c r="F10" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="22">
         <f>SUM($E$2:E10)/$E$23</f>
         <v>0.6</v>
       </c>
-      <c r="J10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <f>A10</f>
         <v>45607</v>
@@ -1108,21 +1071,15 @@
       <c r="E11" s="22">
         <v>2</v>
       </c>
-      <c r="F11" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="17">
-        <v>3</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="10">
+      <c r="F11" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="22">
         <f>SUM($E$2:E11)/$E$23</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <f>A11+7</f>
         <v>45614</v>
@@ -1134,27 +1091,16 @@
       <c r="C12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="22">
-        <v>2</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="17">
-        <v>2</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="10">
+      <c r="D12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="G12" s="28">
         <f>SUM($E$2:E12)/$E$23</f>
-        <v>0.73333333333333328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <f>A12</f>
         <v>45614</v>
@@ -1166,25 +1112,21 @@
       <c r="C13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>16</v>
+      <c r="D13" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="E13" s="22">
         <v>2</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="17">
-        <v>2</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="10">
+      <c r="F13" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="22">
         <f>SUM($E$2:E13)/$E$23</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <f>A13+7</f>
         <v>45621</v>
@@ -1202,24 +1144,15 @@
       <c r="E14" s="22">
         <v>2</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="17">
-        <v>3</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="10">
+      <c r="F14" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="22">
         <f>SUM($E$2:E14)/$E$23</f>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="J14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <f>A14</f>
         <v>45621</v>
@@ -1237,20 +1170,13 @@
       <c r="E15" s="22">
         <v>2</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="10">
+      <c r="F15" s="29"/>
+      <c r="G15" s="22">
         <f>SUM($E$2:E15)/$E$23</f>
-        <v>0.93333333333333335</v>
-      </c>
-      <c r="J15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <f>A15+7</f>
         <v>45628</v>
@@ -1262,22 +1188,21 @@
       <c r="C16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="10">
-        <f>SUM($E$2:E17)/$E$23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="22">
+        <v>2</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="22">
+        <f>SUM($E$2:E16)/$E$23</f>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <f>A16</f>
         <v>45628</v>
@@ -1289,25 +1214,19 @@
       <c r="C17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>1</v>
+      <c r="D17" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E17" s="22">
         <v>2</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="10">
+      <c r="F17" s="29"/>
+      <c r="G17" s="22">
         <f>SUM($E$2:E17)/$E$23</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <f>A17+7</f>
         <v>45635</v>
@@ -1319,20 +1238,12 @@
       <c r="C18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="10">
+      <c r="G18" s="22">
         <f>SUM($E$2:E18)/$E$23</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <f>A18</f>
         <v>45635</v>
@@ -1345,19 +1256,12 @@
         <v>49</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="10">
+      <c r="G19" s="22">
         <f>SUM($E$2:E19)/$E$23</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <f>A19+7</f>
         <v>45642</v>
@@ -1369,14 +1273,8 @@
       <c r="C20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <f>A20</f>
         <v>45642</v>
@@ -1388,14 +1286,8 @@
       <c r="C21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1404,7 +1296,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1412,13 +1304,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E32" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="colorScale" priority="1">
@@ -1432,16 +1324,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1 D1:D15 D17:D19 E23 D23:D1048576">
+  <conditionalFormatting sqref="F1 E23 D23:D1048576 D19 D1:D17">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Theory"</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{A52683A8-AE0E-47A6-9596-30CB0C91B49A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1450,24 +1339,24 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" style="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.453125" style="9" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.26953125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1499,7 +1388,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45580</v>
       </c>
@@ -1530,7 +1419,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <f>A2</f>
         <v>45580</v>
@@ -1565,7 +1454,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <f>A3+7</f>
         <v>45587</v>
@@ -1600,7 +1489,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <f>A3+8</f>
         <v>45588</v>
@@ -1635,7 +1524,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>45601</v>
       </c>
@@ -1669,7 +1558,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <f>A6</f>
         <v>45601</v>
@@ -1701,7 +1590,7 @@
         <v>0.43333333333333335</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <f>A7+7</f>
         <v>45608</v>
@@ -1733,7 +1622,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <f>A8</f>
         <v>45608</v>
@@ -1768,7 +1657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <f>A9+7</f>
         <v>45615</v>
@@ -1803,7 +1692,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <f>A10</f>
         <v>45615</v>
@@ -1835,7 +1724,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <f>A11+7</f>
         <v>45622</v>
@@ -1867,7 +1756,7 @@
         <v>0.76666666666666672</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <f>A12</f>
         <v>45622</v>
@@ -1897,7 +1786,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <f>A13+7</f>
         <v>45629</v>
@@ -1932,7 +1821,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <f>A14</f>
         <v>45629</v>
@@ -1963,7 +1852,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <f>A15+7</f>
         <v>45636</v>
@@ -1990,7 +1879,7 @@
         <v>1.0333333333333334</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <f>A16</f>
         <v>45636</v>
@@ -2020,7 +1909,7 @@
         <v>1.0333333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <f>A17+7</f>
         <v>45643</v>
@@ -2045,7 +1934,7 @@
         <v>1.0333333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <f>A18</f>
         <v>45643</v>
@@ -2070,7 +1959,7 @@
         <v>1.0333333333333334</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <f>A19+7</f>
         <v>45650</v>
@@ -2089,7 +1978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <f>A20</f>
         <v>45650</v>
@@ -2108,7 +1997,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
@@ -2117,7 +2006,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
@@ -2125,7 +2014,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E32" s="24"/>
     </row>
   </sheetData>
@@ -2163,22 +2052,22 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G1" sqref="G1:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="9"/>
+    <col min="4" max="4" width="7.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="9"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2204,7 +2093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>44860</v>
       </c>
@@ -2232,7 +2121,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>44860</v>
       </c>
@@ -2256,7 +2145,7 @@
       </c>
       <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>44867</v>
       </c>
@@ -2282,7 +2171,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>44867</v>
       </c>
@@ -2310,7 +2199,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>44874</v>
       </c>
@@ -2336,7 +2225,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>44874</v>
       </c>
@@ -2364,7 +2253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>44881</v>
       </c>
@@ -2390,7 +2279,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>44881</v>
       </c>
@@ -2418,7 +2307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>44888</v>
       </c>
@@ -2443,7 +2332,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>44888</v>
       </c>
@@ -2468,7 +2357,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>44893</v>
       </c>
@@ -2494,7 +2383,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>44895</v>
       </c>
@@ -2518,7 +2407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>44895</v>
       </c>
@@ -2540,7 +2429,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>44900</v>
       </c>
@@ -2566,7 +2455,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>44902</v>
       </c>
@@ -2592,7 +2481,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>44907</v>
       </c>
@@ -2618,7 +2507,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C18" s="5" t="s">
         <v>2</v>
       </c>

</xml_diff>